<commit_message>
Practica 1: se agrego deteccion de anomalias
</commit_message>
<xml_diff>
--- a/estaturas.xlsx
+++ b/estaturas.xlsx
@@ -4,25 +4,26 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="normales" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="anomalias" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="valtest(normales)" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="anomalias" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjQFgdYEtCGRHBjEAyagaECBq3uXA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjOFKBXFP2zMj4PbmxFo6uUWE2Snw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
-    <t>Estatura</t>
+    <t>Estatura(metros)</t>
   </si>
   <si>
-    <t>Edad</t>
+    <t>Edad(años)</t>
   </si>
   <si>
     <t>1.77</t>
@@ -79,10 +80,16 @@
     <t>1.68</t>
   </si>
   <si>
+    <t>1.60</t>
+  </si>
+  <si>
     <t>1.61</t>
   </si>
   <si>
-    <t>1.60</t>
+    <t>Estatura</t>
+  </si>
+  <si>
+    <t>Edad</t>
   </si>
   <si>
     <t>0.25</t>
@@ -135,10 +142,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -160,6 +167,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -380,226 +391,226 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>26.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>31.0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>24.0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>34.0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>32.0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>29.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>27.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>34.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>26.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>21.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>23.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>25.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>24.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>25.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>25.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>34.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>26.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>25.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>26.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>27.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>32.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>40.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>25.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>24.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>38.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>34.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>29.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>28.0</v>
       </c>
     </row>
@@ -611,54 +622,12 @@
         <v>27.0</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="3">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="5">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="5">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="5">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="5">
-        <v>27.0</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="3">
-        <v>31.0</v>
-      </c>
-    </row>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -1637,48 +1606,135 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5">
+        <v>31.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="5">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5">
+        <v>31.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5">
+        <v>31.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="6" width="14.43"/>
     <col customWidth="1" min="7" max="26" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
+      <c r="A2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="6">
         <v>43557.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
+      <c r="A3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="6">
         <v>43587.0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2">
         <v>250.0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>150.0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>14.0</v>
       </c>
     </row>

</xml_diff>